<commit_message>
Quiero tu beso en la mejilla
</commit_message>
<xml_diff>
--- a/P2-EJ2-DevOps.xlsx
+++ b/P2-EJ2-DevOps.xlsx
@@ -4,8 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Requisitos" sheetId="1" r:id="rId5"/>
-    <sheet state="visible" name="Planificación" sheetId="2" r:id="rId6"/>
-    <sheet state="visible" name="Estimación" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="PE" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="159">
   <si>
     <t>RequisitoID</t>
   </si>
@@ -175,13 +174,328 @@
   </si>
   <si>
     <t>S: Define dos opciones técnicas claras de seguridad.</t>
+  </si>
+  <si>
+    <t>ID Tarea</t>
+  </si>
+  <si>
+    <t>Req.</t>
+  </si>
+  <si>
+    <t>Descripción de la Tarea</t>
+  </si>
+  <si>
+    <t>Dependencias</t>
+  </si>
+  <si>
+    <t>Estimación (SP)</t>
+  </si>
+  <si>
+    <t>G1-01</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Configuración de repositorio Git y estrategia de ramas (Gitflow).</t>
+  </si>
+  <si>
+    <t>Gestión</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>G1-02</t>
+  </si>
+  <si>
+    <t>Configuración de entorno Docker para base de datos y Python.</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>RF1-01</t>
+  </si>
+  <si>
+    <t>Desarrollar parser CSV y mapeo de campos a entidades del sistema.</t>
+  </si>
+  <si>
+    <t>Implementación</t>
+  </si>
+  <si>
+    <t>RF1-02</t>
+  </si>
+  <si>
+    <t>Unit tests: Verificación de tipos de datos e integridad del CSV.</t>
+  </si>
+  <si>
+    <t>Verificación</t>
+  </si>
+  <si>
+    <t>RF1-03</t>
+  </si>
+  <si>
+    <t>Integrar persistencia de datos en base de datos (SQL/NoSQL).</t>
+  </si>
+  <si>
+    <t>Integración</t>
+  </si>
+  <si>
+    <t>RF1-04</t>
+  </si>
+  <si>
+    <t>Documentar el esquema de base de datos y proceso de carga.</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>RF2-01</t>
+  </si>
+  <si>
+    <t>Implementar filtro lógico para aceptar exclusivamente método "GET".</t>
+  </si>
+  <si>
+    <t>RF2-02</t>
+  </si>
+  <si>
+    <t>Test funcional: Enviar peticiones POST/PUT y validar rechazo.</t>
+  </si>
+  <si>
+    <t>RF3-01</t>
+  </si>
+  <si>
+    <t>Implementar lógica de validación de status HTTP (200 y 206).</t>
+  </si>
+  <si>
+    <t>RF3-02</t>
+  </si>
+  <si>
+    <t>Validar que estados fuera de rango (404, 500) sean descartados.</t>
+  </si>
+  <si>
+    <t>RF4-01</t>
+  </si>
+  <si>
+    <t>Crear detector de Bots basado en Regex para el User Agent.</t>
+  </si>
+  <si>
+    <t>RF4-02</t>
+  </si>
+  <si>
+    <t>Testear cadenas "CRAWLER", "SPIDER" y validar detección positiva.</t>
+  </si>
+  <si>
+    <t>RF5-01</t>
+  </si>
+  <si>
+    <t>Implementar validador de extensión ".mp3" en la URI del recurso.</t>
+  </si>
+  <si>
+    <t>RF5-02</t>
+  </si>
+  <si>
+    <t>Testear extensiones prohibidas (.wav, .mp4) y validar error.</t>
+  </si>
+  <si>
+    <t>VAL-INT</t>
+  </si>
+  <si>
+    <t>RF-2..5</t>
+  </si>
+  <si>
+    <t>Integrar todos los filtros en un pipeline de validación secuencial.</t>
+  </si>
+  <si>
+    <t>VAL-DOC</t>
+  </si>
+  <si>
+    <t>Documentar reglas de validación y limpieza de datos en el manual.</t>
+  </si>
+  <si>
+    <t>RF6-01</t>
+  </si>
+  <si>
+    <t>Lógica de generación de observaciones de error con ID y métrica.</t>
+  </si>
+  <si>
+    <t>RF6-02</t>
+  </si>
+  <si>
+    <t>Testear que los errores "Bad method" y "Bot detected" se creen bien.</t>
+  </si>
+  <si>
+    <t>RF6-03</t>
+  </si>
+  <si>
+    <t>Integrar almacenamiento de logs de error en la base de datos.</t>
+  </si>
+  <si>
+    <t>RF6-04</t>
+  </si>
+  <si>
+    <t>Documentar el catálogo de métricas de error disponibles.</t>
+  </si>
+  <si>
+    <t>RF7-01</t>
+  </si>
+  <si>
+    <t>Algoritmo de acumulación de bytes por usuario y umbrales (1MB/30MB).</t>
+  </si>
+  <si>
+    <t>RF7-02</t>
+  </si>
+  <si>
+    <t>Testear generación de "Download 200" al superar el umbral exacto.</t>
+  </si>
+  <si>
+    <t>RF7-03</t>
+  </si>
+  <si>
+    <t>Integrar asignación aleatoria de CCAA (lat/long) a observaciones.</t>
+  </si>
+  <si>
+    <t>RF7-04</t>
+  </si>
+  <si>
+    <t>Documentar lógica de "Usuario Único" (ID + User Agent).</t>
+  </si>
+  <si>
+    <t>RF8-01</t>
+  </si>
+  <si>
+    <t>Desarrollar motor de cálculo de sumatorios para estadísticas.</t>
+  </si>
+  <si>
+    <t>RF8-02</t>
+  </si>
+  <si>
+    <t>Verificar precisión de contadores comparando con datos de prueba.</t>
+  </si>
+  <si>
+    <t>RF8-03</t>
+  </si>
+  <si>
+    <t>Integrar cálculo de estadísticas al final del proceso de carga.</t>
+  </si>
+  <si>
+    <t>RF8-04</t>
+  </si>
+  <si>
+    <t>Documentar el formato de salida del resumen estadístico.</t>
+  </si>
+  <si>
+    <t>RF9-01</t>
+  </si>
+  <si>
+    <t>Implementar algoritmo de ranking Top-K basado en descargas.</t>
+  </si>
+  <si>
+    <t>RF9-02</t>
+  </si>
+  <si>
+    <t>Testear que la lista se ordene de mayor a menor descargas.</t>
+  </si>
+  <si>
+    <t>RF9-03</t>
+  </si>
+  <si>
+    <t>Integrar ranking con la capa de persistencia para consultas rápidas.</t>
+  </si>
+  <si>
+    <t>RF9-04</t>
+  </si>
+  <si>
+    <t>Documentar el uso del parámetro dinámico 'K'.</t>
+  </si>
+  <si>
+    <t>RF10-01</t>
+  </si>
+  <si>
+    <t>Crear componente visual de gráfico de columnas para el Top-K.</t>
+  </si>
+  <si>
+    <t>RF10-02</t>
+  </si>
+  <si>
+    <t>Test de renderizado del gráfico con datos vacíos y con datos.</t>
+  </si>
+  <si>
+    <t>RF10-03</t>
+  </si>
+  <si>
+    <t>Integrar visualización en el frontend o herramienta de BI.</t>
+  </si>
+  <si>
+    <t>RF11-01</t>
+  </si>
+  <si>
+    <t>Programar el flujo de 5 pasos para el sistema de recomendación.</t>
+  </si>
+  <si>
+    <t>RF11-02</t>
+  </si>
+  <si>
+    <t>Verificar que las recomendaciones coincidan con los temas del usuario.</t>
+  </si>
+  <si>
+    <t>RF11-03</t>
+  </si>
+  <si>
+    <t>Integrar sistema de recomendación como servicio independiente.</t>
+  </si>
+  <si>
+    <t>RF11-04</t>
+  </si>
+  <si>
+    <t>Documentar la lógica del algoritmo de recomendación paso a paso.</t>
+  </si>
+  <si>
+    <t>RFN1-01</t>
+  </si>
+  <si>
+    <t>Desarrollar API REST con especificación OpenAPI (Swagger).</t>
+  </si>
+  <si>
+    <t>RF11-03, RF9-03</t>
+  </si>
+  <si>
+    <t>RFN1-02</t>
+  </si>
+  <si>
+    <t>Unit tests de endpoints CRUD para Podcasts y Episodios.</t>
+  </si>
+  <si>
+    <t>RFN1-03</t>
+  </si>
+  <si>
+    <t>Documentar el API utilizando Swagger UI.</t>
+  </si>
+  <si>
+    <t>RFN2-01</t>
+  </si>
+  <si>
+    <t>Implementar autenticación básica o JWT para asegurar el API.</t>
+  </si>
+  <si>
+    <t>RFN2-02</t>
+  </si>
+  <si>
+    <t>Test de intrusión básico: Validar acceso denegado sin credenciales.</t>
+  </si>
+  <si>
+    <t>CI-01</t>
+  </si>
+  <si>
+    <t>Configurar Pipeline de Integración Continua (GitHub Actions).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -197,6 +511,14 @@
       <sz val="11.0"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Google Sans Flex&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="&quot;Google Sans Text&quot;"/>
+    </font>
+    <font>
+      <color rgb="FF1F1F1F"/>
+      <name val="&quot;Google Sans Text&quot;"/>
     </font>
   </fonts>
   <fills count="3">
@@ -219,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -227,6 +549,21 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -288,8 +625,14 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="2">
     <tableStyle count="4" pivot="0" name="Requisitos-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="4" size="0" type="wholeTable"/>
+    </tableStyle>
+    <tableStyle count="4" pivot="0" name="PE-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
@@ -307,10 +650,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
@@ -325,6 +664,20 @@
     <tableColumn name="Metrika" id="5"/>
   </tableColumns>
   <tableStyleInfo name="Requisitos-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F46" displayName="Tabla_2" name="Tabla_2" id="2">
+  <tableColumns count="6">
+    <tableColumn name="ID Tarea" id="1"/>
+    <tableColumn name="Req." id="2"/>
+    <tableColumn name="Descripción de la Tarea" id="3"/>
+    <tableColumn name="Tipo" id="4"/>
+    <tableColumn name="Dependencias" id="5"/>
+    <tableColumn name="Estimación (SP)" id="6"/>
+  </tableColumns>
+  <tableStyleInfo name="PE-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -567,7 +920,7 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -584,7 +937,7 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -601,7 +954,7 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -618,7 +971,7 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -635,7 +988,7 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -652,7 +1005,7 @@
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -669,7 +1022,7 @@
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -686,7 +1039,7 @@
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -703,7 +1056,7 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -720,7 +1073,7 @@
       <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -737,7 +1090,7 @@
       <c r="C12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -754,7 +1107,7 @@
       <c r="C13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -771,7 +1124,7 @@
       <c r="C14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -779,6 +1132,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D14">
+      <formula1>"Funcional,No Funcional"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -792,24 +1150,951 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="37.63"/>
+    <col customWidth="1" min="4" max="4" width="18.0"/>
+    <col customWidth="1" min="5" max="5" width="16.38"/>
+    <col customWidth="1" min="6" max="6" width="20.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" ht="22.5" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" ht="22.5" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4" ht="22.5" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6" ht="22.5" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="7" ht="22.5" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8" ht="22.5" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9" ht="22.5" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10" ht="22.5" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11" ht="22.5" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" ht="22.5" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="13" ht="22.5" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="14" ht="22.5" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="15" ht="22.5" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" ht="22.5" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17" ht="22.5" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" ht="22.5" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19" ht="22.5" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="20" ht="22.5" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="21" ht="22.5" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" ht="22.5" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="7">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="23" ht="22.5" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="24" ht="22.5" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="25" ht="22.5" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="26" ht="22.5" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="27" ht="22.5" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="28" ht="22.5" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="29" ht="22.5" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30" ht="22.5" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="31" ht="22.5" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="32" ht="22.5" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="33" ht="22.5" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34" ht="22.5" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="35" ht="22.5" customHeight="1">
+      <c r="A35" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="36" ht="22.5" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="37" ht="22.5" customHeight="1">
+      <c r="A37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="7">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="38" ht="22.5" customHeight="1">
+      <c r="A38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="39" ht="22.5" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="40" ht="22.5" customHeight="1">
+      <c r="A40" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="41" ht="22.5" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="7">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="42" ht="22.5" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="43" ht="22.5" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="7">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="44" ht="22.5" customHeight="1">
+      <c r="A44" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F44" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="45" ht="22.5" customHeight="1">
+      <c r="A45" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="7">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="46" ht="22.5" customHeight="1">
+      <c r="A46" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="D2:D46">
+      <formula1>"Gestión,DevOps,Implementación,Verificación,Integración,Documentación"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="F2:F46">
+      <formula1>AND(ISNUMBER(F2),(NOT(OR(NOT(ISERROR(DATEVALUE(F2))), AND(ISNUMBER(F2), LEFT(CELL("format", F2))="D")))))</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>